<commit_message>
update pusbin perhitungan nilai
</commit_message>
<xml_diff>
--- a/uploads/nilai/contoh_nilai.xlsx
+++ b/uploads/nilai/contoh_nilai.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonisetiabudi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/bpkp/uploads/nilai/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="77">
   <si>
     <t>KD_EVENT</t>
   </si>
@@ -203,9 +200,6 @@
     <t>03</t>
   </si>
   <si>
-    <t xml:space="preserve">T-258     </t>
-  </si>
-  <si>
     <t>220501</t>
   </si>
   <si>
@@ -258,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">SAPUTRA                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasdsa    </t>
   </si>
 </sst>
 </file>
@@ -576,7 +573,7 @@
   <dimension ref="A1:BE14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +762,7 @@
         <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -774,160 +771,160 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Z2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AQ2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AR2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AS2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AX2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AZ2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BC2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BE2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.2">
@@ -938,7 +935,7 @@
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D3">
         <v>101</v>
@@ -947,160 +944,160 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AQ3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AR3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AS3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AX3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AZ3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BC3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.2">
@@ -1111,7 +1108,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D4">
         <v>102</v>
@@ -1120,160 +1117,160 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AQ4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AR4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AS4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AX4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AZ4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BC4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BE4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.2">
@@ -1284,7 +1281,7 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D5">
         <v>103</v>
@@ -1293,160 +1290,160 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
         <v>67</v>
       </c>
-      <c r="G5" t="s">
-        <v>68</v>
-      </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AH5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AI5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AN5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AP5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AQ5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AR5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AU5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BA5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BE5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.2">
@@ -1457,7 +1454,7 @@
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D6">
         <v>104</v>
@@ -1466,160 +1463,160 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AN6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AR6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AW6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BA6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BD6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BE6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.2">
@@ -1630,7 +1627,7 @@
         <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D7">
         <v>105</v>
@@ -1639,160 +1636,160 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AI7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AN7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AR7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AT7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AW7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BA7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BD7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.2">
@@ -1803,7 +1800,7 @@
         <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D8">
         <v>106</v>
@@ -1812,160 +1809,160 @@
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AH8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AR8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AT8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AZ8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BA8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BD8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BE8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.2">
@@ -1976,7 +1973,7 @@
         <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D9">
         <v>107</v>
@@ -1985,160 +1982,160 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AH9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AI9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AN9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AO9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AR9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AW9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BA9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BC9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BD9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.2">
@@ -2149,7 +2146,7 @@
         <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D10">
         <v>108</v>
@@ -2158,160 +2155,160 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AH10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AI10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AN10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AR10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BA10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BE10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.2">
@@ -2322,7 +2319,7 @@
         <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D11">
         <v>101</v>
@@ -2331,160 +2328,160 @@
         <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AH11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AN11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AO11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AP11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AR11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BA11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.2">
@@ -2495,7 +2492,7 @@
         <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>110</v>
@@ -2504,160 +2501,160 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AQ12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AR12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AS12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AX12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AZ12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BC12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BE12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.2">
@@ -2667,8 +2664,8 @@
       <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="C13">
-        <v>123</v>
+      <c r="C13" t="s">
+        <v>76</v>
       </c>
       <c r="D13">
         <v>111</v>
@@ -2677,160 +2674,160 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AH13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AI13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AN13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AP13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AR13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AT13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AZ13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BA13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BD13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.2">
@@ -2840,8 +2837,8 @@
       <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="C14">
-        <v>123</v>
+      <c r="C14" t="s">
+        <v>76</v>
       </c>
       <c r="D14">
         <v>112</v>
@@ -2850,160 +2847,160 @@
         <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AD14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AF14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AK14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AO14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AQ14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AR14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AT14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AZ14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BA14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BC14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BD14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>